<commit_message>
Deployment of (at least one) server works
</commit_message>
<xml_diff>
--- a/attic/RZ_zuhause/ServerKauf.xlsx
+++ b/attic/RZ_zuhause/ServerKauf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Kauf" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,196 +15,208 @@
     <sheet name="Config" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="247">
-  <si>
-    <t>Gesamt</t>
-  </si>
-  <si>
-    <t>Ges HE</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>HE</t>
-  </si>
-  <si>
-    <t>verfügbar</t>
-  </si>
-  <si>
-    <t>Preis</t>
-  </si>
-  <si>
-    <t>Versand</t>
-  </si>
-  <si>
-    <t>eBay-Nr</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>Platte</t>
-  </si>
-  <si>
-    <t>DVD</t>
-  </si>
-  <si>
-    <t>HP DL380 G5 2x Intel Xeon Quad Core E5450 3GHz 32GB RAM 292GB HDD</t>
-  </si>
-  <si>
-    <t>2x QC</t>
-  </si>
-  <si>
-    <t>3 GHz</t>
-  </si>
-  <si>
-    <t>32 GB</t>
-  </si>
-  <si>
-    <t>2 x 146 GB
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="249">
+  <si>
+    <t xml:space="preserve">Gesamt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ges HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verfügbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eBay-Nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP DL380 G5 2x Intel Xeon Quad Core E5450 3GHz 32GB RAM 292GB HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 146 GB
 10 k SAS</t>
   </si>
   <si>
-    <t>262130635574</t>
-  </si>
-  <si>
-    <t>HP Proliant DL360 G5 Server &gt;&gt; 1x Intel Xeon L5420, 16 GB, 2x 72 GB SAS, Rails</t>
-  </si>
-  <si>
-    <t>1x QC</t>
-  </si>
-  <si>
-    <t>2.5 GHz</t>
-  </si>
-  <si>
-    <t>16 GB</t>
-  </si>
-  <si>
-    <t>2 x 72 GB
+    <t xml:space="preserve">262130635574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Proliant DL360 G5 Server &gt;&gt; 1x Intel Xeon L5420, 16 GB, 2x 72 GB SAS, Rails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 72 GB
 10 k SAS</t>
   </si>
   <si>
-    <t>201483019768</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 - 2X XEON QUAD 3GHz 16GB DDR2 Ram, 2X 146GB SAS HDDs</t>
-  </si>
-  <si>
-    <t>3,00 GHz</t>
-  </si>
-  <si>
-    <t>DVD?</t>
-  </si>
-  <si>
-    <t>Preis in Pfund</t>
-  </si>
-  <si>
-    <t>221752172618</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 2x Xeon QC X5450 3,00GHz 16 GB RAM P400i Raid 146 GB HDD</t>
-  </si>
-  <si>
-    <t>2x 73 GB</t>
-  </si>
-  <si>
-    <t>381462385775</t>
-  </si>
-  <si>
-    <t>HP Proliant DL360 G5 / 1x Xeon E5420 QC @ 2.50GHz / 4GB / 1x72GB,4x146GB / Combo</t>
-  </si>
-  <si>
-    <t>4 GB</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>381494310493</t>
-  </si>
-  <si>
-    <t>4 x 146 GB
+    <t xml:space="preserve">201483019768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 - 2X XEON QUAD 3GHz 16GB DDR2 Ram, 2X 146GB SAS HDDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,00 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVD?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preis in Pfund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221752172618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 2x Xeon QC X5450 3,00GHz 16 GB RAM P400i Raid 146 GB HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 73 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">381462385775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Proliant DL360 G5 / 1x Xeon E5420 QC @ 2.50GHz / 4GB / 1x72GB,4x146GB / Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">381494310493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 x 146 GB
 1 x 72 GB
 10 k SAS</t>
   </si>
   <si>
-    <t>+ Platten, Preis
+    <t xml:space="preserve">+ Platten, Preis
 - 4 GB</t>
   </si>
   <si>
-    <t>321959096749</t>
-  </si>
-  <si>
-    <t>HP Proliant DL360 G5 - 8GB - HDD 2x 146 GB und 2x 72 GB, gebraucht</t>
-  </si>
-  <si>
-    <t>1 x DC</t>
-  </si>
-  <si>
-    <t>2.0 GHz</t>
-  </si>
-  <si>
-    <t>8 GB</t>
-  </si>
-  <si>
-    <t>2 x 146 GB
+    <t xml:space="preserve">321959096749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Proliant DL360 G5 - 8GB - HDD 2x 146 GB und 2x 72 GB, gebraucht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 146 GB
 2 x 72 GB
 10 k SAS</t>
   </si>
   <si>
-    <t>252144301971</t>
-  </si>
-  <si>
-    <t>Server HP DL360 G5 Intel Xeon Quad Core E5405 @ 2 x 2.0Ghz 16GB RAM ohne HDD</t>
-  </si>
-  <si>
-    <t>2,00 GHz</t>
-  </si>
-  <si>
-    <t>252223533478</t>
-  </si>
-  <si>
-    <t>HP Proliant DL360 G5 Server (Intel Xeon QuadCore E5420, 8 GB RAM, 2x 72 GB HDD)</t>
-  </si>
-  <si>
-    <t>161018762577</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 1x Xeon L5335 QC 2.0 GHz, 8 GB RAM, 292 GB SAS 10k</t>
-  </si>
-  <si>
-    <t>151034362956</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 2x Xeon 5130 DC 2.0 GHz, 8 GB RAM, 292 GB SAS</t>
-  </si>
-  <si>
-    <t>2x DC</t>
-  </si>
-  <si>
-    <t>161888359870</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 2x Xeon 5140 DC 2.33 GHz, 8 GB RAM, 292 GB SAS 10k</t>
-  </si>
-  <si>
-    <t>2,33 GHz</t>
-  </si>
-  <si>
-    <t>2x 146 GB
+    <t xml:space="preserve">252144301971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server HP DL360 G5 Intel Xeon Quad Core E5405 @ 2 x 2.0Ghz 16GB RAM ohne HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,00 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">252223533478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Proliant DL360 G5 Server (Intel Xeon QuadCore E5420, 8 GB RAM, 2x 72 GB HDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161018762577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 1x Xeon L5335 QC 2.0 GHz, 8 GB RAM, 292 GB SAS 10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151034362956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 2x Xeon 5130 DC 2.0 GHz, 8 GB RAM, 292 GB SAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161888359870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 2x Xeon 5140 DC 2.33 GHz, 8 GB RAM, 292 GB SAS 10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,33 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 146 GB
 10k SAS</t>
   </si>
   <si>
-    <t>191759984738</t>
+    <t xml:space="preserve">191759984738</t>
   </si>
   <si>
     <r>
-      <t>HP Proliant DL360</t>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP Proliant DL360</t>
     </r>
     <r>
       <rPr>
@@ -215,7 +227,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>G6</t>
+      <t xml:space="preserve">G6</t>
     </r>
     <r>
       <rPr>
@@ -225,575 +237,581 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>XEON QC E5540 2.53GHz 6GB 2x72GB 15K P410i 2x GB-LAN 43</t>
+      <t xml:space="preserve">XEON QC E5540 2.53GHz 6GB 2x72GB 15K P410i 2x GB-LAN 43</t>
     </r>
   </si>
   <si>
-    <t>2,53 GHz</t>
-  </si>
-  <si>
-    <t>6 GB</t>
-  </si>
-  <si>
-    <t>2 x 72 GB
+    <t xml:space="preserve">2,53 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 72 GB
 15 k SAS</t>
   </si>
   <si>
-    <t>+ G6, 15k HDD
+    <t xml:space="preserve">+ G6, 15k HDD
 - 6 GB</t>
   </si>
   <si>
-    <t>321667542682</t>
-  </si>
-  <si>
-    <t>HP ProLiant DL360 G5 2x Xeon QC E5450 3,00GHz 32 GB RAM P400i Raid</t>
-  </si>
-  <si>
-    <t>272035328819</t>
-  </si>
-  <si>
-    <t>HP Proliant DL360 G6 Server // 1x E5520, 12 GB, 2x 72 GB, P410i, 1x PSU, Rails</t>
-  </si>
-  <si>
-    <t>2,26 GHz</t>
-  </si>
-  <si>
-    <t>12 GB</t>
-  </si>
-  <si>
-    <t>+ G6, 15k HDD
+    <t xml:space="preserve">321667542682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP ProLiant DL360 G5 2x Xeon QC E5450 3,00GHz 32 GB RAM P400i Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272035328819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Proliant DL360 G6 Server // 1x E5520, 12 GB, 2x 72 GB, P410i, 1x PSU, Rails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,26 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ G6, 15k HDD
 - Preis</t>
   </si>
   <si>
-    <t>Netzwerk</t>
-  </si>
-  <si>
-    <t>9 Server</t>
-  </si>
-  <si>
-    <t>18 Gbit</t>
-  </si>
-  <si>
-    <t>2 LAN</t>
-  </si>
-  <si>
-    <t>9 100MBit</t>
-  </si>
-  <si>
-    <t>1 ILO</t>
-  </si>
-  <si>
-    <t>112 cm</t>
-  </si>
-  <si>
-    <t>28 HE</t>
-  </si>
-  <si>
-    <t>12 HE</t>
-  </si>
-  <si>
-    <t>Serverschrank 76 x 60 x 60 cm</t>
-  </si>
-  <si>
-    <t>15 HE</t>
-  </si>
-  <si>
-    <t>Serverschrank Netzwerkschrank Netzwerk LANscape</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ILO</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Typ</t>
-  </si>
-  <si>
-    <t>CPU</t>
-  </si>
-  <si>
-    <t>Ghz</t>
-  </si>
-  <si>
-    <t>Platte 1</t>
-  </si>
-  <si>
-    <t>Platte 2</t>
-  </si>
-  <si>
-    <t>Platte 3</t>
-  </si>
-  <si>
-    <t>Platte 4</t>
-  </si>
-  <si>
-    <t>Platte 5</t>
-  </si>
-  <si>
-    <t>LEVEL</t>
-  </si>
-  <si>
-    <t>ergibt</t>
-  </si>
-  <si>
-    <t>Links 1 (Watt)</t>
-  </si>
-  <si>
-    <t>Links 2 (Watt)</t>
-  </si>
-  <si>
-    <t>Rechts 1</t>
-  </si>
-  <si>
-    <t>Rechts 2</t>
-  </si>
-  <si>
-    <t>NEUTRAL</t>
-  </si>
-  <si>
-    <t>example.com</t>
-  </si>
-  <si>
-    <t>172.16.1.0/24</t>
-  </si>
-  <si>
-    <t>172.16.10.0/24</t>
-  </si>
-  <si>
-    <t>WLAN</t>
-  </si>
-  <si>
-    <t>LAN</t>
-  </si>
-  <si>
-    <t>Bildschirm</t>
-  </si>
-  <si>
-    <t>jump</t>
-  </si>
-  <si>
-    <t>1xQC 2.5GHz 16GB</t>
-  </si>
-  <si>
-    <t>RAID 5</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>rhev11</t>
-  </si>
-  <si>
-    <t>rhev21</t>
-  </si>
-  <si>
-    <t>rhev12</t>
-  </si>
-  <si>
-    <t>2xQC 3.0GHz 16GB</t>
-  </si>
-  <si>
-    <t>rhev22</t>
-  </si>
-  <si>
-    <t>gluster11</t>
-  </si>
-  <si>
-    <t>gluster21</t>
-  </si>
-  <si>
-    <t>gluster12</t>
-  </si>
-  <si>
-    <t>2xQC 3.0GHz 32GB</t>
-  </si>
-  <si>
-    <t>gluster22</t>
-  </si>
-  <si>
-    <t>RHEVM</t>
-  </si>
-  <si>
-    <t>Watt</t>
-  </si>
-  <si>
-    <t>Ampere</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>Sicherung</t>
-  </si>
-  <si>
-    <t>Querschnitt</t>
-  </si>
-  <si>
-    <t>max. Leistung</t>
-  </si>
-  <si>
-    <t>mx. Länge</t>
-  </si>
-  <si>
-    <t>16 A</t>
-  </si>
-  <si>
-    <t>1,5 mm²</t>
-  </si>
-  <si>
-    <t>3680 Watt</t>
-  </si>
-  <si>
-    <t>18,11 m</t>
-  </si>
-  <si>
-    <t>13 A</t>
-  </si>
-  <si>
-    <t>2990 Watt</t>
-  </si>
-  <si>
-    <t>22,29 m</t>
-  </si>
-  <si>
-    <t>10 A</t>
-  </si>
-  <si>
-    <t>2300 Watt</t>
-  </si>
-  <si>
-    <t>28,98 m</t>
-  </si>
-  <si>
-    <t>2,5 mm²</t>
-  </si>
-  <si>
-    <t>30,19 m</t>
-  </si>
-  <si>
-    <t>37,15 m</t>
-  </si>
-  <si>
-    <t>48,30 m</t>
-  </si>
-  <si>
-    <t>0,5mm² = 3 A/690W</t>
-  </si>
-  <si>
-    <t>0,75 mm² = 6 A/1380W</t>
-  </si>
-  <si>
-    <t>1 mm² = 10 A/2300W</t>
-  </si>
-  <si>
-    <t>1,5 mm² = 16 A/3600W</t>
-  </si>
-  <si>
-    <t>2,5 mm2 = 25 A/5750W</t>
-  </si>
-  <si>
-    <t>1,5 mm²  –  10/13 Ampere</t>
-  </si>
-  <si>
-    <t>2,5 mm²  –   16 Ampere</t>
-  </si>
-  <si>
-    <t>4    mm²  –   20 Ampere</t>
-  </si>
-  <si>
-    <t>6    mm²  –   25 Ampere</t>
-  </si>
-  <si>
-    <t>10  mm²  –   40 Ampere</t>
-  </si>
-  <si>
-    <t>16  mm²  –   63 Ampere</t>
-  </si>
-  <si>
-    <t>25  mm²  –   80 Ampere</t>
-  </si>
-  <si>
-    <t>35  mm²  – 100 Ampere</t>
-  </si>
-  <si>
-    <t>Was</t>
-  </si>
-  <si>
-    <t>Geplant</t>
-  </si>
-  <si>
-    <t>IST</t>
-  </si>
-  <si>
-    <t>Kosten</t>
-  </si>
-  <si>
-    <t>ebay</t>
-  </si>
-  <si>
-    <t>jereist</t>
-  </si>
-  <si>
-    <t>compicool</t>
-  </si>
-  <si>
-    <t>uk conmputerparts wembley</t>
-  </si>
-  <si>
-    <t>pars-computer</t>
-  </si>
-  <si>
-    <t>Ersatzserver</t>
-  </si>
-  <si>
-    <t>ixustrade</t>
-  </si>
-  <si>
-    <t>zeughouse</t>
-  </si>
-  <si>
-    <t>CAT 7 Kabel</t>
-  </si>
-  <si>
-    <t>amazon</t>
-  </si>
-  <si>
-    <t>Stromleisten (Brennenstuhl Super-Solid Line 8-fach silber mit Schalter, 1153340118)</t>
-  </si>
-  <si>
-    <t>WLAN (1240E + 1000E) + 1240E</t>
-  </si>
-  <si>
-    <t>Serverschrank</t>
-  </si>
-  <si>
-    <t>andreas4822</t>
-  </si>
-  <si>
-    <t>Fachboden</t>
-  </si>
-  <si>
-    <t>HP NC360T Dual Port, PCI Express x4, Full Profile, SP 412651-001</t>
-  </si>
-  <si>
-    <t>bert-ley</t>
-  </si>
-  <si>
-    <t>Schrauben</t>
-  </si>
-  <si>
-    <t>Serverschienen</t>
-  </si>
-  <si>
-    <t>Stromleisten (4* 8er Brennstuhl für 100 €) (3* 10er Brennstuhl für 74€)</t>
-  </si>
-  <si>
-    <t>Discovery</t>
-  </si>
-  <si>
-    <t>base deployment</t>
-  </si>
-  <si>
-    <t>All Hosts</t>
-  </si>
-  <si>
-    <t>Content Host</t>
-  </si>
-  <si>
-    <t>katello_agent</t>
-  </si>
-  <si>
-    <t>Sub-mgr list</t>
-  </si>
-  <si>
-    <t>now</t>
-  </si>
-  <si>
-    <t>gluster install</t>
-  </si>
-  <si>
-    <t>Filesysteme in GB</t>
-  </si>
-  <si>
-    <t>172.16.20.0/24</t>
-  </si>
-  <si>
-    <t>ORIGINAL</t>
-  </si>
-  <si>
-    <t>jump.example.com</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>config</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>swap</t>
-  </si>
-  <si>
-    <t>DC1</t>
-  </si>
-  <si>
-    <t>00:1B:78:76:98:BE</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>10 MB</t>
-  </si>
-  <si>
-    <t>00:1E:0B:EC:33:F0</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>1.5x RAM + 512 MB</t>
-  </si>
-  <si>
-    <t>RAM*0.5 + 4GB</t>
-  </si>
-  <si>
-    <t>00:1E:0B:91:D6:D2</t>
-  </si>
-  <si>
-    <t>7.1 + gluster 3.1</t>
-  </si>
-  <si>
-    <t>100 MB</t>
-  </si>
-  <si>
-    <t>00:1C:C4:DD:D3:0E</t>
-  </si>
-  <si>
-    <t>7.2 + gluster 3.1</t>
-  </si>
-  <si>
-    <t>DC2</t>
-  </si>
-  <si>
-    <t>00:1C:C4:A6:9C:3A</t>
-  </si>
-  <si>
-    <t>00:1E:0B:5F:EA:34</t>
-  </si>
-  <si>
-    <t>00:1E:0B:91:92:B6</t>
-  </si>
-  <si>
-    <t>7.2 Beta</t>
-  </si>
-  <si>
-    <t>00:1F:29:E6:B4:84</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>25 bis 50 GB</t>
-  </si>
-  <si>
-    <t>my local LAN</t>
-  </si>
-  <si>
-    <t>192.168.2.0/24</t>
-  </si>
-  <si>
-    <t>192.168.188.0/24</t>
-  </si>
-  <si>
-    <t>speedport</t>
-  </si>
-  <si>
-    <t>dhcp, dns</t>
-  </si>
-  <si>
-    <t>does not find it's drive within linux</t>
-  </si>
-  <si>
-    <t>fritz.box</t>
-  </si>
-  <si>
-    <t>Approaches:</t>
-  </si>
-  <si>
-    <t>homematic</t>
-  </si>
-  <si>
-    <t>change the RAID-Baterie – mentioned to be low</t>
-  </si>
-  <si>
-    <t>jupiter</t>
-  </si>
-  <si>
-    <t>use the “Offline HPE Smart Storage Administrator (HPE SSA)” to find misconfiguration</t>
-  </si>
-  <si>
-    <t>Samsung Drucker</t>
-  </si>
-  <si>
-    <t>dhcp</t>
-  </si>
-  <si>
-    <t>Hpssaoffline-2 → burn ISO and run</t>
-  </si>
-  <si>
-    <t>jump ILO</t>
-  </si>
-  <si>
-    <t>E200 Firmware</t>
-  </si>
-  <si>
-    <t>via Smart Update Firmware DVD</t>
-  </si>
-  <si>
-    <t>switch1</t>
-  </si>
-  <si>
-    <t>powerline</t>
-  </si>
-  <si>
-    <t>http://h20564.www2.hpe.com/hpsc/swd/public/readIndex?sp4ts.oid=1121413&amp;swLangOid=8&amp;swEnvOid=4103</t>
-  </si>
-  <si>
-    <t>ntp via dhcp setzen</t>
-  </si>
-  <si>
-    <t>sync_hwclock yes in /etc/sysconfig/ntpdate</t>
-  </si>
-  <si>
-    <t>jump in /etc/ntp/step-tickers eintragen</t>
-  </si>
-  <si>
-    <t>ntpd enablen</t>
+    <t xml:space="preserve">Netzwerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Gbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 100MBit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">112 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serverschrank 76 x 60 x 60 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serverschrank Netzwerkschrank Netzwerk LANscape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platte 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ergibt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links 1 (Watt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links 2 (Watt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechts 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechts 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEUTRAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.1.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.10.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildschirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1xQC 2.5GHz 16GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAID 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhev11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhev21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhev12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2xQC 3.0GHz 16GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhev22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gluster11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gluster21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gluster12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2xQC 3.0GHz 32GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gluster22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHEVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicherung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Querschnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. Leistung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mx. Länge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 mm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3680 Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,11 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2990 Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22,29 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300 Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,98 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5 mm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,19 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,15 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48,30 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5mm² = 3 A/690W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,75 mm² = 6 A/1380W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 mm² = 10 A/2300W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 mm² = 16 A/3600W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5 mm2 = 25 A/5750W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 mm²  –  10/13 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5 mm²  –   16 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4    mm²  –   20 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6    mm²  –   25 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10  mm²  –   40 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16  mm²  –   63 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25  mm²  –   80 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35  mm²  – 100 Ampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geplant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kosten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ebay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jereist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compicool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk conmputerparts wembley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pars-computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersatzserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ixustrade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zeughouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT 7 Kabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stromleisten (Brennenstuhl Super-Solid Line 8-fach silber mit Schalter, 1153340118)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WLAN (1240E + 1000E) + 1240E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serverschrank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andreas4822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachboden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP NC360T Dual Port, PCI Express x4, Full Profile, SP 412651-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bert-ley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schrauben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serverschienen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stromleisten (4* 8er Brennstuhl für 100 €) (3* 10er Brennstuhl für 74€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Hosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">katello_agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-mgr list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gluster install</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filesysteme in GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.20.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORIGINAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jump.example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1B:78:76:98:BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1E:0B:EC:33:F0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5x RAM + 512 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAM*0.5 + 4GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1E:0B:91:D6:D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.1 + gluster 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1C:C4:DD:D3:0E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2 + gluster 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1C:C4:A6:9C:3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1E:0B:5F:EA:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1E:0B:91:92:B6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2 Beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:1F:29:E6:B4:84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 bis 50 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my local LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.2.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.188.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speedport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhcp, dns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">does not find it's drive within linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fritz.box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approaches:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homematic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change the RAID-Baterie – mentioned to be low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jupiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use the “Offline HPE Smart Storage Administrator (HPE SSA)” to find misconfiguration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Drucker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhcp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hpssaoffline-2 → burn ISO and run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jump ILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E200 Firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">via Smart Update Firmware DVD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://h20564.www2.hpe.com/hpsc/swd/public/readIndex?sp4ts.oid=1121413&amp;swLangOid=8&amp;swEnvOid=4103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntp via dhcp setzen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sync_hwclock yes in /etc/sysconfig/ntpdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jump in /etc/ntp/step-tickers eintragen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntpd enablen</t>
   </si>
 </sst>
 </file>
@@ -801,7 +819,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="* #,##0.00&quot; € &quot;;\-* #,##0.00&quot; € &quot;;* \-#&quot; € &quot;;@\ "/>
     <numFmt numFmtId="166" formatCode="* #,##0&quot;  HE&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
@@ -921,7 +939,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1136,15 +1154,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="36.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1967,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1970,19 +1988,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.8520408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.14795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,7 +2697,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2700,7 +2718,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +2956,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2959,12 +2977,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="7"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="7.14795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3484,7 +3502,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3500,18 +3518,18 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,6 +3654,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="B6" s="0" t="s">
         <v>113</v>
       </c>
@@ -3643,7 +3664,7 @@
         <v>102</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>102</v>
@@ -3661,16 +3682,16 @@
         <v>201</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>7.2</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,7 +3702,7 @@
         <v>103</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>103</v>
@@ -3699,19 +3720,19 @@
         <v>201</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M7" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>50</v>
@@ -3728,7 +3749,7 @@
         <v>104</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>104</v>
@@ -3752,11 +3773,11 @@
         <v>7.2</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M8" s="32"/>
       <c r="O8" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>50</v>
@@ -3767,7 +3788,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>112</v>
@@ -3776,7 +3797,7 @@
         <v>201</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>201</v>
@@ -3801,6 +3822,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>217</v>
+      </c>
       <c r="B11" s="0" t="s">
         <v>115</v>
       </c>
@@ -3808,7 +3832,7 @@
         <v>202</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>202</v>
@@ -3840,7 +3864,7 @@
         <v>203</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>203</v>
@@ -3858,14 +3882,14 @@
         <v>201</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M12" s="32"/>
       <c r="O12" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>50</v>
@@ -3882,7 +3906,7 @@
         <v>204</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>204</v>
@@ -3900,14 +3924,14 @@
         <v>201</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M13" s="32"/>
       <c r="O13" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>50</v>
@@ -3918,7 +3942,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L15" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,29 +3950,29 @@
         <v>121</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>33</v>
@@ -3957,12 +3981,12 @@
         <v>117</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>110</v>
@@ -3971,12 +3995,12 @@
         <v>1</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2</v>
@@ -3985,15 +4009,15 @@
         <v>2</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>10</v>
@@ -4002,29 +4026,29 @@
         <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>111</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>101</v>
@@ -4033,10 +4057,10 @@
         <v>101</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4050,60 +4074,60 @@
         <v>102</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>110</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
added dhcp and dns for ilo systems
</commit_message>
<xml_diff>
--- a/attic/RZ_zuhause/ServerKauf.xlsx
+++ b/attic/RZ_zuhause/ServerKauf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Kauf" sheetId="1" state="visible" r:id="rId2"/>
@@ -1146,7 +1146,7 @@
   </sheetPr>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1154,15 +1154,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,19 +1988,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,7 +2718,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,12 +2977,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3517,22 +3517,25 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>512912</v>
+      </c>
       <c r="C1" s="0" t="s">
         <v>84</v>
       </c>

</xml_diff>